<commit_message>
add airNow/ cultral resources; split i-tree; update glossary
</commit_message>
<xml_diff>
--- a/siteGeneration/glossary.xlsx
+++ b/siteGeneration/glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klr324/Documents/Github/climToolsReference/siteGeneration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD48B6DE-CB63-6C49-9BC8-823410243BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EE0F82-2550-8142-862C-6966D4215072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1180" windowWidth="26660" windowHeight="14400" xr2:uid="{5E01B77E-7114-AA48-84BB-2B0608713F1C}"/>
+    <workbookView xWindow="2140" yWindow="2480" windowWidth="26660" windowHeight="14400" xr2:uid="{5E01B77E-7114-AA48-84BB-2B0608713F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>keyword</t>
   </si>
@@ -169,9 +169,6 @@
     <t>Carbon Emissions</t>
   </si>
   <si>
-    <t>Only Tools Related To Coasts</t>
-  </si>
-  <si>
     <t>Registration required</t>
   </si>
   <si>
@@ -289,9 +286,6 @@
     <t>(tag) The tool provides estimated costs.</t>
   </si>
   <si>
-    <t>(tag) The tool provides a one or more solutions.</t>
-  </si>
-  <si>
     <t>(tag) The tool allows the user to compare multiple scenarios or locations.</t>
   </si>
   <si>
@@ -310,9 +304,6 @@
     <t>(tag) The tool contains information as a website. It may or may not be interactive.</t>
   </si>
   <si>
-    <t>(tag) The information in the tool is specific to one or more location.</t>
-  </si>
-  <si>
     <t>(tag) The information in the tool is at the watershed level.</t>
   </si>
   <si>
@@ -496,9 +487,6 @@
     <t>(tool function) Visualizing or comparing possible future scenarios projected by climate models.</t>
   </si>
   <si>
-    <t>(geographic scope) Coastal counties are counties adjacent to the open ocean, major estuaries, and the Great Lakes where they are exposed to a range of coastal hazards and host economic production associated with coastal and ocean resources. Coastal counties can also be counties where land use and water quality changes directly impact coastal ecosystems.</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -509,6 +497,36 @@
   </si>
   <si>
     <t>Varies</t>
+  </si>
+  <si>
+    <t>Cultural Resources</t>
+  </si>
+  <si>
+    <t>(coastal / inland) Tools that consist of noncoastal or inland topics.</t>
+  </si>
+  <si>
+    <t>(coastal / inland) Tools that consist of coastal topics.</t>
+  </si>
+  <si>
+    <t>Coastal</t>
+  </si>
+  <si>
+    <t>Noncoastal/ Inland</t>
+  </si>
+  <si>
+    <t>(tag) The tool provides one or more solutions.</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>(tag) The tool is an application.</t>
+  </si>
+  <si>
+    <t>(tag) The information in the tool is specific to one or more locations.</t>
+  </si>
+  <si>
+    <t>(society) Any prehistoric or historic remains or indicators of past human activities, including artifacts, sites, structures, landscapes, and objects of importance to a culture or community for scientific, traditional, religious, or other reasons. Culture resources in this tool also encompass tools that illustrate recent/current human opinions, beliefs, or behaviors.</t>
   </si>
 </sst>
 </file>
@@ -911,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DFD664-A791-3E44-AAE8-83790EB19B95}">
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -956,7 +974,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -964,7 +982,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -972,7 +990,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -980,7 +998,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -988,7 +1006,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -996,7 +1014,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1004,7 +1022,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1012,7 +1030,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1020,7 +1038,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1028,7 +1046,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1036,7 +1054,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1044,7 +1062,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1052,7 +1070,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1060,7 +1078,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1082,7 +1100,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1104,7 +1122,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1112,7 +1130,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1120,7 +1138,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1128,7 +1146,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1150,7 +1168,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1172,7 +1190,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1180,7 +1198,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1202,7 +1220,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1224,7 +1242,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1243,10 +1261,10 @@
     </row>
     <row r="27" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1254,7 +1272,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -1262,197 +1280,183 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+    </row>
+    <row r="33" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
+    <row r="34" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="7" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+    </row>
+    <row r="35" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-    </row>
-    <row r="32" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="3" t="s">
+    </row>
+    <row r="36" spans="1:16" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-    </row>
-    <row r="34" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
     </row>
     <row r="37" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
+      <c r="B43" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="44" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -1469,49 +1473,63 @@
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
     </row>
-    <row r="45" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>153</v>
-      </c>
+    <row r="45" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
     </row>
     <row r="46" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>45</v>
+      <c r="A46" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>104</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>46</v>
+      <c r="A47" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>103</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>99</v>
@@ -1519,47 +1537,47 @@
     </row>
     <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>94</v>
@@ -1567,47 +1585,47 @@
     </row>
     <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>88</v>
@@ -1615,7 +1633,7 @@
     </row>
     <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>87</v>
@@ -1623,130 +1641,154 @@
     </row>
     <row r="64" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>63</v>
+        <v>160</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>86</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="8" t="s">
-        <v>72</v>
+      <c r="A73" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>154</v>
+      <c r="A76" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>155</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>156</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>157</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>